<commit_message>
caracteristica scrappeo de competiciones, posibilidad de actualizacion e insercion de nueva temporada si hay campeon, scrappear_partidos dividido en varios archivos py
</commit_message>
<xml_diff>
--- a/Crear database/partidos.xlsx
+++ b/Crear database/partidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1539,6 +1539,120 @@
         <v>317</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">21:00 </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Atletico de Madrid</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1–3</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>César Soto</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>1883</v>
+      </c>
+      <c r="H30" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-01-29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">16:15 </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Atletico de Madrid</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1–0</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>CA Osasuna</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Alberola Rojas</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>624</v>
+      </c>
+      <c r="H31" t="n">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-02-04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18:30 </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Atletico de Madrid</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1–1</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Getafe CF</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Antonio Matéu</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>2830</v>
+      </c>
+      <c r="H32" t="n">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>